<commit_message>
Changing strings to identify A* and A conferences (before it was AA and AB, respectively)
</commit_message>
<xml_diff>
--- a/data/phase3-results-groupedPerCORERank.xlsx
+++ b/data/phase3-results-groupedPerCORERank.xlsx
@@ -352,10 +352,10 @@
     <t>C</t>
   </si>
   <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>AA</t>
+    <t>A*</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,7 +973,7 @@
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <v>57.166666666666664</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>37</v>

</xml_diff>

<commit_message>
Explaining what you will find in the EXCEL files
</commit_message>
<xml_diff>
--- a/data/phase3-results-groupedPerCORERank.xlsx
+++ b/data/phase3-results-groupedPerCORERank.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="results_24Feb_B" localSheetId="0">Hoja1!$A$1:$BY$104</definedName>
+    <definedName name="results_24Feb_B" localSheetId="0">Hoja1!$A$1:$AY$104</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Rank</t>
   </si>
@@ -250,94 +250,16 @@
     <t>Community_Papers</t>
   </si>
   <si>
-    <t>AvgDegree_1_LastEdition</t>
-  </si>
-  <si>
-    <t>AvgDegree_2_LastEdition</t>
-  </si>
-  <si>
-    <t>AvgDegree_3_LastEdition</t>
-  </si>
-  <si>
-    <t>AvgDegree_4_LastEdition</t>
-  </si>
-  <si>
-    <t>AvgDegree_5_LastEdition</t>
-  </si>
-  <si>
     <t>Avg_Degree</t>
   </si>
   <si>
-    <t>GraphDensity_1_LastEdition</t>
-  </si>
-  <si>
-    <t>GraphDensity_2_LastEdition</t>
-  </si>
-  <si>
-    <t>GraphDensity_3_LastEdition</t>
-  </si>
-  <si>
-    <t>GraphDensity_4_LastEdition</t>
-  </si>
-  <si>
-    <t>GraphDensity_5_LastEdition</t>
-  </si>
-  <si>
     <t>Graph_Density</t>
   </si>
   <si>
-    <t>GraphModularity_1_LastEdition</t>
-  </si>
-  <si>
-    <t>GraphModularity_2_LastEdition</t>
-  </si>
-  <si>
-    <t>GraphModularity_3_LastEdition</t>
-  </si>
-  <si>
-    <t>GraphModularity_4_LastEdition</t>
-  </si>
-  <si>
-    <t>GraphModularity_5_LastEdition</t>
-  </si>
-  <si>
     <t>Graph_Modularity</t>
   </si>
   <si>
-    <t>ConnectedComponents_1_LastEdition</t>
-  </si>
-  <si>
-    <t>ConnectedComponents_2_LastEdition</t>
-  </si>
-  <si>
-    <t>ConnectedComponents_3_LastEdition</t>
-  </si>
-  <si>
-    <t>ConnectedComponents_4_LastEdition</t>
-  </si>
-  <si>
-    <t>ConnectedComponents_5_LastEdition</t>
-  </si>
-  <si>
     <t>Connected_Components</t>
-  </si>
-  <si>
-    <t>AveragePathLength_1_LastEdition</t>
-  </si>
-  <si>
-    <t>AveragePathLength_2_LastEdition</t>
-  </si>
-  <si>
-    <t>AveragePathLength_3_LastEdition</t>
-  </si>
-  <si>
-    <t>AveragePathLength_4_LastEdition</t>
-  </si>
-  <si>
-    <t>AveragePathLength_5_LastEdition</t>
-  </si>
-  <si>
-    <t>Avg_Path_Length</t>
   </si>
   <si>
     <t>Prominent_Figures</t>
@@ -698,11 +620,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BY5"/>
+  <dimension ref="A1:AY5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="AZ33" sqref="AZ33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,21 +646,15 @@
     <col min="40" max="40" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="41" max="44" width="29" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="50" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12" bestFit="1" customWidth="1"/>
-    <col min="52" max="56" width="26" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="14" bestFit="1" customWidth="1"/>
-    <col min="58" max="62" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="68" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="74" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="18" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -892,88 +808,10 @@
       <c r="AY1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" t="s">
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>53</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>79</v>
       </c>
       <c r="B2">
         <v>57.166666666666664</v>
@@ -1108,105 +946,27 @@
         <v>7.0954999999999986</v>
       </c>
       <c r="AT2">
-        <v>4.3952480794280726</v>
+        <v>4.9489229048700087</v>
       </c>
       <c r="AU2">
-        <v>4.2426100514912184</v>
+        <v>7.360351718400264E-3</v>
       </c>
       <c r="AV2">
-        <v>3.9852087225375139</v>
+        <v>99.083333333333329</v>
       </c>
       <c r="AW2">
-        <v>3.8146585635617747</v>
+        <v>90.583333333333329</v>
       </c>
       <c r="AX2">
-        <v>3.9636635370973448</v>
+        <v>1.8239166666666666</v>
       </c>
       <c r="AY2">
-        <v>4.9489229048700087</v>
-      </c>
-      <c r="AZ2">
-        <v>2.2125518928721891E-2</v>
-      </c>
-      <c r="BA2">
-        <v>2.4014144850649118E-2</v>
-      </c>
-      <c r="BB2">
-        <v>2.4008597553617159E-2</v>
-      </c>
-      <c r="BC2">
-        <v>2.5311209165132093E-2</v>
-      </c>
-      <c r="BD2">
-        <v>2.6528452165326066E-2</v>
-      </c>
-      <c r="BE2">
-        <v>7.360351718400264E-3</v>
-      </c>
-      <c r="BF2">
-        <v>44</v>
-      </c>
-      <c r="BG2">
-        <v>43.833333333333336</v>
-      </c>
-      <c r="BH2">
-        <v>42.333333333333336</v>
-      </c>
-      <c r="BI2">
-        <v>37.833333333333336</v>
-      </c>
-      <c r="BJ2">
-        <v>38.25</v>
-      </c>
-      <c r="BK2">
-        <v>99.083333333333329</v>
-      </c>
-      <c r="BL2">
-        <v>43.583333333333336</v>
-      </c>
-      <c r="BM2">
-        <v>43.166666666666664</v>
-      </c>
-      <c r="BN2">
-        <v>41.916666666666664</v>
-      </c>
-      <c r="BO2">
-        <v>37.333333333333336</v>
-      </c>
-      <c r="BP2">
-        <v>38</v>
-      </c>
-      <c r="BQ2">
-        <v>90.583333333333329</v>
-      </c>
-      <c r="BR2">
-        <v>1.4338925305167234</v>
-      </c>
-      <c r="BS2">
-        <v>1.5582408348382881</v>
-      </c>
-      <c r="BT2">
-        <v>1.4230605710994118</v>
-      </c>
-      <c r="BU2">
-        <v>1.4574375107176376</v>
-      </c>
-      <c r="BV2">
-        <v>1.3588207328088868</v>
-      </c>
-      <c r="BW2">
-        <v>5.1110101362223928</v>
-      </c>
-      <c r="BX2">
-        <v>1.8239166666666666</v>
-      </c>
-      <c r="BY2">
         <v>734.16666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>37</v>
@@ -1341,105 +1101,27 @@
         <v>7.3028620689655179</v>
       </c>
       <c r="AT3">
-        <v>3.2411579624816516</v>
+        <v>3.5532132358483164</v>
       </c>
       <c r="AU3">
-        <v>3.0916025557648017</v>
+        <v>9.8555028663598783E-3</v>
       </c>
       <c r="AV3">
-        <v>3.2728739631230277</v>
+        <v>84.551724137931032</v>
       </c>
       <c r="AW3">
-        <v>2.8573280706228634</v>
+        <v>82.275862068965523</v>
       </c>
       <c r="AX3">
-        <v>2.8867695621910148</v>
+        <v>1.1906896551724138</v>
       </c>
       <c r="AY3">
-        <v>3.5532132358483164</v>
-      </c>
-      <c r="AZ3">
-        <v>3.4740087760340148E-2</v>
-      </c>
-      <c r="BA3">
-        <v>3.5768807118751932E-2</v>
-      </c>
-      <c r="BB3">
-        <v>3.8100461725035034E-2</v>
-      </c>
-      <c r="BC3">
-        <v>3.6450473580070086E-2</v>
-      </c>
-      <c r="BD3">
-        <v>3.614110190371761E-2</v>
-      </c>
-      <c r="BE3">
-        <v>9.8555028663598783E-3</v>
-      </c>
-      <c r="BF3">
-        <v>30.310344827586206</v>
-      </c>
-      <c r="BG3">
-        <v>27.206896551724139</v>
-      </c>
-      <c r="BH3">
-        <v>25.758620689655171</v>
-      </c>
-      <c r="BI3">
-        <v>26.482758620689655</v>
-      </c>
-      <c r="BJ3">
-        <v>27.03448275862069</v>
-      </c>
-      <c r="BK3">
-        <v>84.551724137931032</v>
-      </c>
-      <c r="BL3">
-        <v>30.172413793103448</v>
-      </c>
-      <c r="BM3">
-        <v>27.103448275862068</v>
-      </c>
-      <c r="BN3">
-        <v>25.586206896551722</v>
-      </c>
-      <c r="BO3">
-        <v>26.413793103448278</v>
-      </c>
-      <c r="BP3">
-        <v>27</v>
-      </c>
-      <c r="BQ3">
-        <v>82.275862068965523</v>
-      </c>
-      <c r="BR3">
-        <v>1.2498330291119841</v>
-      </c>
-      <c r="BS3">
-        <v>1.1907621924429856</v>
-      </c>
-      <c r="BT3">
-        <v>1.2373183066748139</v>
-      </c>
-      <c r="BU3">
-        <v>1.1657776775009197</v>
-      </c>
-      <c r="BV3">
-        <v>1.1871619184062754</v>
-      </c>
-      <c r="BW3">
-        <v>2.6875967579159412</v>
-      </c>
-      <c r="BX3">
-        <v>1.1906896551724138</v>
-      </c>
-      <c r="BY3">
         <v>419.86206896551727</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>34.953488372093027</v>
@@ -1574,105 +1256,27 @@
         <v>7.7008139534883719</v>
       </c>
       <c r="AT4">
-        <v>3.2176637510999968</v>
+        <v>3.4912999818059101</v>
       </c>
       <c r="AU4">
-        <v>3.1117021952587192</v>
+        <v>1.0062858271940546E-2</v>
       </c>
       <c r="AV4">
-        <v>2.7920223216481723</v>
+        <v>101.93023255813954</v>
       </c>
       <c r="AW4">
-        <v>2.8127334729941915</v>
+        <v>100.34883720930233</v>
       </c>
       <c r="AX4">
-        <v>3.5088088813058662</v>
+        <v>1.174209302325582</v>
       </c>
       <c r="AY4">
-        <v>3.4912999818059101</v>
-      </c>
-      <c r="AZ4">
-        <v>4.0616426771018059E-2</v>
-      </c>
-      <c r="BA4">
-        <v>4.1072809702248955E-2</v>
-      </c>
-      <c r="BB4">
-        <v>3.5920975122078959E-2</v>
-      </c>
-      <c r="BC4">
-        <v>3.9417895049865655E-2</v>
-      </c>
-      <c r="BD4">
-        <v>4.1651443062068687E-2</v>
-      </c>
-      <c r="BE4">
-        <v>1.0062858271940546E-2</v>
-      </c>
-      <c r="BF4">
-        <v>28.744186046511629</v>
-      </c>
-      <c r="BG4">
-        <v>29.953488372093023</v>
-      </c>
-      <c r="BH4">
-        <v>31.093023255813954</v>
-      </c>
-      <c r="BI4">
-        <v>29.348837209302324</v>
-      </c>
-      <c r="BJ4">
-        <v>31.302325581395348</v>
-      </c>
-      <c r="BK4">
-        <v>101.93023255813954</v>
-      </c>
-      <c r="BL4">
-        <v>28.581395348837209</v>
-      </c>
-      <c r="BM4">
-        <v>29.767441860465116</v>
-      </c>
-      <c r="BN4">
-        <v>30.906976744186046</v>
-      </c>
-      <c r="BO4">
-        <v>29.302325581395348</v>
-      </c>
-      <c r="BP4">
-        <v>31.209302325581394</v>
-      </c>
-      <c r="BQ4">
-        <v>100.34883720930233</v>
-      </c>
-      <c r="BR4">
-        <v>1.2183256573963006</v>
-      </c>
-      <c r="BS4">
-        <v>1.2740584037294977</v>
-      </c>
-      <c r="BT4">
-        <v>1.2311139929958173</v>
-      </c>
-      <c r="BU4">
-        <v>1.149987067307392</v>
-      </c>
-      <c r="BV4">
-        <v>1.1864570169610031</v>
-      </c>
-      <c r="BW4">
-        <v>2.1987614055395324</v>
-      </c>
-      <c r="BX4">
-        <v>1.174209302325582</v>
-      </c>
-      <c r="BY4">
         <v>459.37209302325579</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>27.111111111111111</v>
@@ -1807,99 +1411,21 @@
         <v>8.0226666666666677</v>
       </c>
       <c r="AT5">
-        <v>3.51874738634787</v>
+        <v>3.5198127849488947</v>
       </c>
       <c r="AU5">
-        <v>3.1729181001701106</v>
+        <v>1.2084698260523581E-2</v>
       </c>
       <c r="AV5">
-        <v>3.1529268751919557</v>
+        <v>94.833333333333329</v>
       </c>
       <c r="AW5">
-        <v>3.0367102385938209</v>
+        <v>93.111111111111114</v>
       </c>
       <c r="AX5">
-        <v>2.9102419554936105</v>
+        <v>1.7290000000000001</v>
       </c>
       <c r="AY5">
-        <v>3.5198127849488947</v>
-      </c>
-      <c r="AZ5">
-        <v>5.2695152255014671E-2</v>
-      </c>
-      <c r="BA5">
-        <v>4.4857641906020367E-2</v>
-      </c>
-      <c r="BB5">
-        <v>4.652605466106563E-2</v>
-      </c>
-      <c r="BC5">
-        <v>4.2677085265929594E-2</v>
-      </c>
-      <c r="BD5">
-        <v>4.6287541218200258E-2</v>
-      </c>
-      <c r="BE5">
-        <v>1.2084698260523581E-2</v>
-      </c>
-      <c r="BF5">
-        <v>21.611111111111111</v>
-      </c>
-      <c r="BG5">
-        <v>24.055555555555557</v>
-      </c>
-      <c r="BH5">
-        <v>31.722222222222221</v>
-      </c>
-      <c r="BI5">
-        <v>27.333333333333332</v>
-      </c>
-      <c r="BJ5">
-        <v>21.666666666666668</v>
-      </c>
-      <c r="BK5">
-        <v>94.833333333333329</v>
-      </c>
-      <c r="BL5">
-        <v>21.333333333333332</v>
-      </c>
-      <c r="BM5">
-        <v>23.833333333333332</v>
-      </c>
-      <c r="BN5">
-        <v>31.555555555555557</v>
-      </c>
-      <c r="BO5">
-        <v>27.166666666666668</v>
-      </c>
-      <c r="BP5">
-        <v>21.555555555555557</v>
-      </c>
-      <c r="BQ5">
-        <v>93.111111111111114</v>
-      </c>
-      <c r="BR5">
-        <v>1.372132187115026</v>
-      </c>
-      <c r="BS5">
-        <v>1.1913251219440677</v>
-      </c>
-      <c r="BT5">
-        <v>1.2112317237454631</v>
-      </c>
-      <c r="BU5">
-        <v>1.2463880818338373</v>
-      </c>
-      <c r="BV5">
-        <v>1.1917837572964938</v>
-      </c>
-      <c r="BW5">
-        <v>2.3676608759132152</v>
-      </c>
-      <c r="BX5">
-        <v>1.7290000000000001</v>
-      </c>
-      <c r="BY5">
         <v>416.44444444444446</v>
       </c>
     </row>

</xml_diff>